<commit_message>
EOD Change the form of the head to head adding league form
</commit_message>
<xml_diff>
--- a/doc/pourcentageReussitePrediction.xlsx
+++ b/doc/pourcentageReussitePrediction.xlsx
@@ -168,10 +168,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -191,23 +191,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="serie_a_2019-20_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="serie_a_2019-20_2" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="serie_a_2019-20" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="serie_a_2019-20_3" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="premier_league_2018-19" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="serie_a_2019-20_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="serie_a_2019-20_2" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="serie_a_2019-20" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="serie_a_2019-20_3" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -476,7 +476,7 @@
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -487,30 +487,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
     </row>
     <row r="2" spans="1:22" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -531,14 +531,14 @@
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>677</v>
+        <v>703</v>
       </c>
       <c r="C3" s="3">
-        <v>1407</v>
+        <v>1395</v>
       </c>
       <c r="D3" s="4">
         <f>B3/C3*100</f>
-        <v>48.116560056858567</v>
+        <v>50.394265232974909</v>
       </c>
     </row>
     <row r="4" spans="1:22" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -546,14 +546,14 @@
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>672</v>
+        <v>698</v>
       </c>
       <c r="C4" s="3">
-        <v>1407</v>
+        <v>1395</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ref="D4:D11" si="0">B4/C4*100</f>
-        <v>47.761194029850742</v>
+        <v>50.035842293906811</v>
       </c>
     </row>
     <row r="5" spans="1:22" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -561,14 +561,14 @@
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <v>665</v>
+        <v>696</v>
       </c>
       <c r="C5" s="3">
-        <v>1407</v>
+        <v>1395</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" si="0"/>
-        <v>47.263681592039802</v>
+        <v>49.892473118279568</v>
       </c>
     </row>
     <row r="6" spans="1:22" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -576,14 +576,14 @@
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>659</v>
+        <v>695</v>
       </c>
       <c r="C6" s="3">
-        <v>1407</v>
+        <v>1395</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" si="0"/>
-        <v>46.837242359630423</v>
+        <v>49.820788530465947</v>
       </c>
     </row>
     <row r="7" spans="1:22" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -591,14 +591,14 @@
         <v>5</v>
       </c>
       <c r="B7" s="3">
-        <v>654</v>
+        <v>692</v>
       </c>
       <c r="C7" s="3">
-        <v>1407</v>
+        <v>1395</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>46.481876332622605</v>
+        <v>49.605734767025091</v>
       </c>
     </row>
     <row r="8" spans="1:22" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -606,14 +606,14 @@
         <v>6</v>
       </c>
       <c r="B8" s="3">
-        <v>639</v>
+        <v>686</v>
       </c>
       <c r="C8" s="3">
-        <v>1407</v>
+        <v>1395</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="0"/>
-        <v>45.41577825159915</v>
+        <v>49.17562724014337</v>
       </c>
     </row>
     <row r="9" spans="1:22" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -621,14 +621,14 @@
         <v>7</v>
       </c>
       <c r="B9" s="3">
-        <v>639</v>
+        <v>679</v>
       </c>
       <c r="C9" s="3">
-        <v>1407</v>
+        <v>1395</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" si="0"/>
-        <v>45.41577825159915</v>
+        <v>48.673835125448029</v>
       </c>
     </row>
     <row r="10" spans="1:22" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -636,14 +636,14 @@
         <v>8</v>
       </c>
       <c r="B10" s="3">
-        <v>631</v>
+        <v>672</v>
       </c>
       <c r="C10" s="3">
-        <v>1407</v>
+        <v>1395</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" si="0"/>
-        <v>44.847192608386635</v>
+        <v>48.172043010752688</v>
       </c>
     </row>
     <row r="11" spans="1:22" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -651,24 +651,24 @@
         <v>9</v>
       </c>
       <c r="B11" s="3">
-        <v>625</v>
+        <v>671</v>
       </c>
       <c r="C11" s="3">
-        <v>1407</v>
+        <v>1395</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" si="0"/>
-        <v>44.420753375977256</v>
+        <v>48.100358422939067</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A1:D1"/>
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
-    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>